<commit_message>
Inclusion of constraining reference (EVE consensus) into alignment
</commit_message>
<xml_diff>
--- a/tabular/locus/efv-locus-data.xlsx
+++ b/tabular/locus/efv-locus-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/locus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D18F8AD-E994-7D49-BAB9-5A939014B308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C27F07-F536-E64E-B5C1-42E879449C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="600" windowWidth="37080" windowHeight="23280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Done" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4781" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4781" uniqueCount="1090">
   <si>
     <t>sequenceID</t>
   </si>
@@ -3292,6 +3292,18 @@
   </si>
   <si>
     <t>Flavi-like</t>
+  </si>
+  <si>
+    <t>EJV-JMTV1.1.1.1-Chironomus_riparius</t>
+  </si>
+  <si>
+    <t>EJV-JMTV1.1.1.1-Chironomus_tentans</t>
+  </si>
+  <si>
+    <t>EJV-JMTV1.2.1.1-Gerris</t>
+  </si>
+  <si>
+    <t>EJV-JMTV3.1.1.1-Gerris</t>
   </si>
 </sst>
 </file>
@@ -5419,8 +5431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
-      <selection activeCell="P67" sqref="P67:P344"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8929,7 +8941,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
-        <v>42</v>
+        <v>1086</v>
       </c>
       <c r="B63" s="21" t="s">
         <v>290</v>
@@ -8985,7 +8997,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
-        <v>43</v>
+        <v>1087</v>
       </c>
       <c r="B64" s="21" t="s">
         <v>290</v>
@@ -9041,7 +9053,7 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
-        <v>40</v>
+        <v>1088</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>289</v>
@@ -9097,7 +9109,7 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
-        <v>39</v>
+        <v>1089</v>
       </c>
       <c r="B66" s="21" t="s">
         <v>288</v>

</xml_diff>